<commit_message>
unavailable link elimination update
</commit_message>
<xml_diff>
--- a/data/interim/output_links.xlsx
+++ b/data/interim/output_links.xlsx
@@ -1266,7 +1266,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>Failed to connect</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>Failed to connect</t>
         </is>
       </c>
     </row>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>Failed to connect</t>
         </is>
       </c>
     </row>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>Failed to connect</t>
         </is>
       </c>
     </row>
@@ -3346,7 +3346,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>Failed to connect</t>
         </is>
       </c>
     </row>
@@ -3366,7 +3366,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>Failed to connect</t>
         </is>
       </c>
     </row>
@@ -3466,7 +3466,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>Failed to connect</t>
         </is>
       </c>
     </row>

</xml_diff>